<commit_message>
feat: pratical work correction
</commit_message>
<xml_diff>
--- a/0-exercices/ressources/dictionnaire_donnees.xlsx
+++ b/0-exercices/ressources/dictionnaire_donnees.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\formations\coderbase\2itech\cad_merignac_11092023\2-merise\ressources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\formations\coderbase\2itech\cad_merignac_11092023\2-merise\0-exercices\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA750DF4-1391-40F2-B8FB-050A45BA576D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB03383-8FF6-4506-90F3-8A549948BB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-36" windowWidth="25812" windowHeight="14016" xr2:uid="{04B90186-9B0E-4BC1-B8EC-CFA316EDE382}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{04B90186-9B0E-4BC1-B8EC-CFA316EDE382}"/>
   </bookViews>
   <sheets>
-    <sheet name="Données" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="2" r:id="rId1"/>
+    <sheet name="Modele" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="104">
   <si>
     <t>Taille/longueur</t>
   </si>
@@ -67,6 +68,276 @@
   </si>
   <si>
     <t>Bon de commande</t>
+  </si>
+  <si>
+    <t>code postal postal hôtel</t>
+  </si>
+  <si>
+    <t>adresse hôtel</t>
+  </si>
+  <si>
+    <t>nom de l'hôtel</t>
+  </si>
+  <si>
+    <t>ville hôtel</t>
+  </si>
+  <si>
+    <t>nom de la chambre</t>
+  </si>
+  <si>
+    <t>numéro de téléphone de l'hôtel</t>
+  </si>
+  <si>
+    <t>nom de la catégorie</t>
+  </si>
+  <si>
+    <t>numéro de la classe</t>
+  </si>
+  <si>
+    <t>nombre d'étoile</t>
+  </si>
+  <si>
+    <t>identifiant de l'hôtel</t>
+  </si>
+  <si>
+    <t>identifiant de la chambre</t>
+  </si>
+  <si>
+    <t>identifiant de la catégorie</t>
+  </si>
+  <si>
+    <t>tarif de la chambre en fonction de la catégorie</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>enumération restauration, spa, massage, salle de sport, yoga, location de vélo, blanchesserie, autres</t>
+  </si>
+  <si>
+    <t>numéro du service</t>
+  </si>
+  <si>
+    <t>nom_prestation</t>
+  </si>
+  <si>
+    <t>tarif_unit</t>
+  </si>
+  <si>
+    <t>nb_etoiles</t>
+  </si>
+  <si>
+    <t>nom_cat</t>
+  </si>
+  <si>
+    <t>num_cat</t>
+  </si>
+  <si>
+    <t>nom_chamb</t>
+  </si>
+  <si>
+    <t>id_classe</t>
+  </si>
+  <si>
+    <t>id_prestation</t>
+  </si>
+  <si>
+    <t>id_hotel</t>
+  </si>
+  <si>
+    <t>nom_hotel</t>
+  </si>
+  <si>
+    <t>adresse_hotel</t>
+  </si>
+  <si>
+    <t>code_postal_hotel</t>
+  </si>
+  <si>
+    <t>ville_hotel</t>
+  </si>
+  <si>
+    <t>tel_hotel</t>
+  </si>
+  <si>
+    <t>id_chamb</t>
+  </si>
+  <si>
+    <t>identifiant réservation</t>
+  </si>
+  <si>
+    <t>date début de réservation</t>
+  </si>
+  <si>
+    <t>date fin de réservation</t>
+  </si>
+  <si>
+    <t>montant acompte réservation</t>
+  </si>
+  <si>
+    <t>date paiement acompte</t>
+  </si>
+  <si>
+    <t>hypothèse</t>
+  </si>
+  <si>
+    <t>description du service</t>
+  </si>
+  <si>
+    <t>quantité du service</t>
+  </si>
+  <si>
+    <t>date du service</t>
+  </si>
+  <si>
+    <t>identifiant du client</t>
+  </si>
+  <si>
+    <t>nom du client</t>
+  </si>
+  <si>
+    <t>prénom du client</t>
+  </si>
+  <si>
+    <t>adresse client</t>
+  </si>
+  <si>
+    <t>code postale client</t>
+  </si>
+  <si>
+    <t>ville client</t>
+  </si>
+  <si>
+    <t>montant du service</t>
+  </si>
+  <si>
+    <t>prix total du service</t>
+  </si>
+  <si>
+    <t>desc_prestation</t>
+  </si>
+  <si>
+    <t>date_prestation</t>
+  </si>
+  <si>
+    <t>montant_prestation</t>
+  </si>
+  <si>
+    <t>quantite_prestation</t>
+  </si>
+  <si>
+    <t>prix_total</t>
+  </si>
+  <si>
+    <t>donnée calculé</t>
+  </si>
+  <si>
+    <t>quantité * prix unitaire</t>
+  </si>
+  <si>
+    <t>id_reservation</t>
+  </si>
+  <si>
+    <t>date_debut</t>
+  </si>
+  <si>
+    <t>date_fin</t>
+  </si>
+  <si>
+    <t>acompte</t>
+  </si>
+  <si>
+    <t>date_acompte</t>
+  </si>
+  <si>
+    <t>id_client</t>
+  </si>
+  <si>
+    <t>nom_client</t>
+  </si>
+  <si>
+    <t>prenom_client</t>
+  </si>
+  <si>
+    <t>adresse_client</t>
+  </si>
+  <si>
+    <t>code_postale_client</t>
+  </si>
+  <si>
+    <t>ville_client</t>
+  </si>
+  <si>
+    <t>Hors SI</t>
+  </si>
+  <si>
+    <t>Restitution entretien avec le client</t>
+  </si>
+  <si>
+    <t>Ne doit pas apparaître dans la modélisation</t>
+  </si>
+  <si>
+    <t>Facture</t>
+  </si>
+  <si>
+    <t>Photo carte du menu</t>
+  </si>
+  <si>
+    <t>numérique</t>
+  </si>
+  <si>
+    <t>alphanumérique</t>
+  </si>
+  <si>
+    <t>Format des données dans le MCD</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>traduction en anglais du nom de service</t>
+  </si>
+  <si>
+    <t>Hypothèse d'une traduction en dehors, à implémenter dans le programme</t>
+  </si>
+  <si>
+    <t>A deduire par rapport à la description française</t>
+  </si>
+  <si>
+    <t>description_prestation_en</t>
+  </si>
+  <si>
+    <t>5,2 (5 entiers et 2 decimaux)</t>
+  </si>
+  <si>
+    <t>3,2 (3 entiers et 2 decimaux)</t>
+  </si>
+  <si>
+    <t>enumération standard, suite, villa ou prenium</t>
+  </si>
+  <si>
+    <t>num_chamb</t>
+  </si>
+  <si>
+    <t>numero_chambre</t>
+  </si>
+  <si>
+    <t>les deux dernières chiffres ne doivent pas être 13</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>date et heure</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>la date de début doit être avant la date d'arrivée</t>
   </si>
 </sst>
 </file>
@@ -90,12 +361,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -125,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -138,7 +421,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +746,830 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCEF9C4-1566-4006-A927-078DD05D443B}">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="50" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.21875" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="27.21875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="43" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="2">
+        <v>255</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="1">
+        <v>75</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="1">
+        <v>100</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="1">
+        <v>150</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="1">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="1">
+        <v>255</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="1">
+        <v>75</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="1">
+        <v>255</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="1">
+        <v>100</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="1">
+        <v>255</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="1">
+        <v>255</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="1">
+        <v>255</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="1">
+        <v>5</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="7">
+        <v>10</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="1">
+        <v>255</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="1">
+        <v>10</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="1">
+        <v>10</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="7">
+        <v>10</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="1">
+        <v>255</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="1">
+        <v>75</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="1">
+        <v>75</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="1">
+        <v>150</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="1">
+        <v>5</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="1">
+        <v>150</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02378822-8590-4246-BEF4-5FEFDF0632E2}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -493,7 +1607,7 @@
       <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>